<commit_message>
The directory, which separates indicators levels, was created with variables renaming
</commit_message>
<xml_diff>
--- a/private_apps/AI_fiction_or_scientific/result_new.xlsx
+++ b/private_apps/AI_fiction_or_scientific/result_new.xlsx
@@ -381,7 +381,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>6114</v>
+        <v>6000</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -396,7 +396,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>148130</v>
+        <v>163075</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -411,7 +411,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>28673</v>
+        <v>30649</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -426,7 +426,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>19.36</v>
+        <v>18.79</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -441,7 +441,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>24.23</v>
+        <v>27.18</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -456,7 +456,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>6.64</v>
+        <v>7.84</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
The function for calculating frequency of TOP 5 most popular words was created
</commit_message>
<xml_diff>
--- a/private_apps/AI_fiction_or_scientific/result_new.xlsx
+++ b/private_apps/AI_fiction_or_scientific/result_new.xlsx
@@ -381,7 +381,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>6000</v>
+        <v>6114</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -396,7 +396,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>163075</v>
+        <v>148130</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -411,7 +411,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>30649</v>
+        <v>28673</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -426,7 +426,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>18.79</v>
+        <v>19.36</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -441,7 +441,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>27.18</v>
+        <v>24.23</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -456,7 +456,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>7.84</v>
+        <v>6.64</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>

</xml_diff>